<commit_message>
added ratio and proportion
</commit_message>
<xml_diff>
--- a/HTML5/Maths HTML/MATHS-HTML.xlsx
+++ b/HTML5/Maths HTML/MATHS-HTML.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>SNO</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Diret and indirect proportions</t>
+  </si>
+  <si>
+    <t>C6_L11_Ratioandproportions</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,6 +696,14 @@
       </c>
       <c r="B23" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mc6l8datahandling plus and minus functionality completed
</commit_message>
<xml_diff>
--- a/HTML5/Maths HTML/MATHS-HTML.xlsx
+++ b/HTML5/Maths HTML/MATHS-HTML.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>SNO</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>layout pending</t>
+  </si>
+  <si>
+    <t>mc6l8datahandling</t>
+  </si>
+  <si>
+    <t>mc7l5Triangle properties</t>
   </si>
 </sst>
 </file>
@@ -483,11 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,7 +516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -522,7 +527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -533,7 +538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -544,7 +549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -555,7 +560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -566,7 +571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -586,7 +591,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -618,7 +623,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -629,7 +634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -640,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -651,9 +656,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
@@ -662,9 +667,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
@@ -673,9 +678,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -684,9 +689,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
@@ -697,7 +702,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
@@ -714,7 +719,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -725,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -743,6 +748,9 @@
       <c r="B23" t="s">
         <v>25</v>
       </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -755,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -766,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -779,7 +787,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>32</v>
@@ -790,7 +798,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
@@ -799,9 +807,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>34</v>
@@ -810,14 +818,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D29">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="PARTIAL"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D29"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>